<commit_message>
minor fix to yinchuan-bistros
</commit_message>
<xml_diff>
--- a/assets/yinchuan-bistros.xlsx
+++ b/assets/yinchuan-bistros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyeu\leagyun\ningxia-tour\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DB01F-6D59-44C9-BE58-F7819D96D43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDDFC7D-8D0B-4183-AF6F-3C31ECEC69E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="551" yWindow="1478" windowWidth="24042" windowHeight="14500" xr2:uid="{285B717D-0861-472D-B66C-60D5817688A1}"/>
+    <workbookView xWindow="889" yWindow="1816" windowWidth="24042" windowHeight="14500" xr2:uid="{285B717D-0861-472D-B66C-60D5817688A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Eatable" sheetId="2" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.55" x14ac:dyDescent="0.25"/>

</xml_diff>